<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig-2@e7fdb17e6507a83a9549af7fb55b502a0b242442 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-ncpi-bamcram.xlsx
+++ b/StructureDefinition-ncpi-bamcram.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5871" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5869" uniqueCount="581">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-08-12T17:45:57+00:00</t>
+    <t>2025-08-12T18:02:45+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1477,6 +1477,9 @@
     <t>Observation.component:assay_strategy.value[x]</t>
   </si>
   <si>
+    <t>https://nih-ncpi.github.io/ncpi-fhir-ig-2/ValueSet/assay-strategy-vs</t>
+  </si>
+  <si>
     <t>Observation.component:assay_strategy.dataAbsentReason</t>
   </si>
   <si>
@@ -1513,6 +1516,9 @@
   </si>
   <si>
     <t>Observation.component:platform_instrument.value[x]</t>
+  </si>
+  <si>
+    <t>https://nih-ncpi.github.io/ncpi-fhir-ig-2/ValueSet/platform-instrument-vs</t>
   </si>
   <si>
     <t>Observation.component:platform_instrument.dataAbsentReason</t>
@@ -2206,7 +2212,7 @@
     <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="54.6171875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="43.21484375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="57.140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="27.2421875" customWidth="true" bestFit="true"/>
@@ -9173,13 +9179,11 @@
         <v>20</v>
       </c>
       <c r="X58" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y58" t="s" s="2">
-        <v>20</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="Y58" s="2"/>
       <c r="Z58" t="s" s="2">
-        <v>20</v>
+        <v>465</v>
       </c>
       <c r="AA58" t="s" s="2">
         <v>20</v>
@@ -9232,7 +9236,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B59" t="s" s="2">
         <v>449</v>
@@ -9354,7 +9358,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B60" t="s" s="2">
         <v>453</v>
@@ -9476,7 +9480,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B61" t="s" s="2">
         <v>454</v>
@@ -9598,13 +9602,13 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B62" t="s" s="2">
         <v>427</v>
       </c>
       <c r="C62" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="D62" t="s" s="2">
         <v>20</v>
@@ -9722,7 +9726,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B63" t="s" s="2">
         <v>437</v>
@@ -9840,7 +9844,7 @@
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B64" t="s" s="2">
         <v>438</v>
@@ -9960,7 +9964,7 @@
     </row>
     <row r="65">
       <c r="A65" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B65" t="s" s="2">
         <v>439</v>
@@ -10082,7 +10086,7 @@
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B66" t="s" s="2">
         <v>440</v>
@@ -10130,7 +10134,7 @@
         <v>20</v>
       </c>
       <c r="S66" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="T66" t="s" s="2">
         <v>20</v>
@@ -10204,7 +10208,7 @@
     </row>
     <row r="67">
       <c r="A67" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B67" t="s" s="2">
         <v>445</v>
@@ -10267,13 +10271,11 @@
         <v>20</v>
       </c>
       <c r="X67" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y67" t="s" s="2">
-        <v>20</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="Y67" s="2"/>
       <c r="Z67" t="s" s="2">
-        <v>20</v>
+        <v>477</v>
       </c>
       <c r="AA67" t="s" s="2">
         <v>20</v>
@@ -10326,7 +10328,7 @@
     </row>
     <row r="68">
       <c r="A68" t="s" s="2">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B68" t="s" s="2">
         <v>449</v>
@@ -10448,7 +10450,7 @@
     </row>
     <row r="69">
       <c r="A69" t="s" s="2">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B69" t="s" s="2">
         <v>453</v>
@@ -10570,7 +10572,7 @@
     </row>
     <row r="70">
       <c r="A70" t="s" s="2">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B70" t="s" s="2">
         <v>454</v>
@@ -10692,13 +10694,13 @@
     </row>
     <row r="71">
       <c r="A71" t="s" s="2">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B71" t="s" s="2">
         <v>427</v>
       </c>
       <c r="C71" t="s" s="2">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="D71" t="s" s="2">
         <v>20</v>
@@ -10816,7 +10818,7 @@
     </row>
     <row r="72">
       <c r="A72" t="s" s="2">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B72" t="s" s="2">
         <v>437</v>
@@ -10934,7 +10936,7 @@
     </row>
     <row r="73">
       <c r="A73" t="s" s="2">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B73" t="s" s="2">
         <v>438</v>
@@ -11054,7 +11056,7 @@
     </row>
     <row r="74">
       <c r="A74" t="s" s="2">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="B74" t="s" s="2">
         <v>439</v>
@@ -11176,7 +11178,7 @@
     </row>
     <row r="75">
       <c r="A75" t="s" s="2">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B75" t="s" s="2">
         <v>440</v>
@@ -11224,7 +11226,7 @@
         <v>20</v>
       </c>
       <c r="S75" t="s" s="2">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="T75" t="s" s="2">
         <v>20</v>
@@ -11298,7 +11300,7 @@
     </row>
     <row r="76">
       <c r="A76" t="s" s="2">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B76" t="s" s="2">
         <v>445</v>
@@ -11420,7 +11422,7 @@
     </row>
     <row r="77">
       <c r="A77" t="s" s="2">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="B77" t="s" s="2">
         <v>449</v>
@@ -11542,7 +11544,7 @@
     </row>
     <row r="78">
       <c r="A78" t="s" s="2">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B78" t="s" s="2">
         <v>453</v>
@@ -11664,7 +11666,7 @@
     </row>
     <row r="79">
       <c r="A79" t="s" s="2">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="B79" t="s" s="2">
         <v>454</v>
@@ -11786,13 +11788,13 @@
     </row>
     <row r="80">
       <c r="A80" t="s" s="2">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="B80" t="s" s="2">
         <v>427</v>
       </c>
       <c r="C80" t="s" s="2">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="D80" t="s" s="2">
         <v>20</v>
@@ -11910,7 +11912,7 @@
     </row>
     <row r="81">
       <c r="A81" t="s" s="2">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="B81" t="s" s="2">
         <v>437</v>
@@ -12028,7 +12030,7 @@
     </row>
     <row r="82">
       <c r="A82" t="s" s="2">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="B82" t="s" s="2">
         <v>438</v>
@@ -12148,7 +12150,7 @@
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="B83" t="s" s="2">
         <v>439</v>
@@ -12270,7 +12272,7 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="B84" t="s" s="2">
         <v>440</v>
@@ -12318,7 +12320,7 @@
         <v>20</v>
       </c>
       <c r="S84" t="s" s="2">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="T84" t="s" s="2">
         <v>20</v>
@@ -12392,7 +12394,7 @@
     </row>
     <row r="85">
       <c r="A85" t="s" s="2">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="B85" t="s" s="2">
         <v>445</v>
@@ -12514,7 +12516,7 @@
     </row>
     <row r="86">
       <c r="A86" t="s" s="2">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="B86" t="s" s="2">
         <v>449</v>
@@ -12636,7 +12638,7 @@
     </row>
     <row r="87">
       <c r="A87" t="s" s="2">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="B87" t="s" s="2">
         <v>453</v>
@@ -12758,7 +12760,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="2">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="B88" t="s" s="2">
         <v>454</v>
@@ -12880,13 +12882,13 @@
     </row>
     <row r="89">
       <c r="A89" t="s" s="2">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="B89" t="s" s="2">
         <v>427</v>
       </c>
       <c r="C89" t="s" s="2">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="D89" t="s" s="2">
         <v>20</v>
@@ -13004,7 +13006,7 @@
     </row>
     <row r="90">
       <c r="A90" t="s" s="2">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="B90" t="s" s="2">
         <v>437</v>
@@ -13122,7 +13124,7 @@
     </row>
     <row r="91">
       <c r="A91" t="s" s="2">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B91" t="s" s="2">
         <v>438</v>
@@ -13242,7 +13244,7 @@
     </row>
     <row r="92">
       <c r="A92" t="s" s="2">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="B92" t="s" s="2">
         <v>439</v>
@@ -13364,7 +13366,7 @@
     </row>
     <row r="93">
       <c r="A93" t="s" s="2">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B93" t="s" s="2">
         <v>440</v>
@@ -13412,7 +13414,7 @@
         <v>20</v>
       </c>
       <c r="S93" t="s" s="2">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="T93" t="s" s="2">
         <v>20</v>
@@ -13486,7 +13488,7 @@
     </row>
     <row r="94">
       <c r="A94" t="s" s="2">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B94" t="s" s="2">
         <v>445</v>
@@ -13608,7 +13610,7 @@
     </row>
     <row r="95">
       <c r="A95" t="s" s="2">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="B95" t="s" s="2">
         <v>449</v>
@@ -13730,7 +13732,7 @@
     </row>
     <row r="96">
       <c r="A96" t="s" s="2">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B96" t="s" s="2">
         <v>453</v>
@@ -13852,7 +13854,7 @@
     </row>
     <row r="97">
       <c r="A97" t="s" s="2">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="B97" t="s" s="2">
         <v>454</v>
@@ -13974,13 +13976,13 @@
     </row>
     <row r="98">
       <c r="A98" t="s" s="2">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="B98" t="s" s="2">
         <v>427</v>
       </c>
       <c r="C98" t="s" s="2">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="D98" t="s" s="2">
         <v>20</v>
@@ -14098,7 +14100,7 @@
     </row>
     <row r="99">
       <c r="A99" t="s" s="2">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B99" t="s" s="2">
         <v>437</v>
@@ -14216,7 +14218,7 @@
     </row>
     <row r="100">
       <c r="A100" t="s" s="2">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="B100" t="s" s="2">
         <v>438</v>
@@ -14336,7 +14338,7 @@
     </row>
     <row r="101">
       <c r="A101" t="s" s="2">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="B101" t="s" s="2">
         <v>439</v>
@@ -14458,7 +14460,7 @@
     </row>
     <row r="102">
       <c r="A102" t="s" s="2">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="B102" t="s" s="2">
         <v>440</v>
@@ -14506,7 +14508,7 @@
         <v>20</v>
       </c>
       <c r="S102" t="s" s="2">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="T102" t="s" s="2">
         <v>20</v>
@@ -14580,7 +14582,7 @@
     </row>
     <row r="103">
       <c r="A103" t="s" s="2">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="B103" t="s" s="2">
         <v>445</v>
@@ -14702,7 +14704,7 @@
     </row>
     <row r="104">
       <c r="A104" t="s" s="2">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="B104" t="s" s="2">
         <v>449</v>
@@ -14824,7 +14826,7 @@
     </row>
     <row r="105">
       <c r="A105" t="s" s="2">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="B105" t="s" s="2">
         <v>453</v>
@@ -14946,7 +14948,7 @@
     </row>
     <row r="106">
       <c r="A106" t="s" s="2">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="B106" t="s" s="2">
         <v>454</v>
@@ -15068,13 +15070,13 @@
     </row>
     <row r="107">
       <c r="A107" t="s" s="2">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="B107" t="s" s="2">
         <v>427</v>
       </c>
       <c r="C107" t="s" s="2">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="D107" t="s" s="2">
         <v>20</v>
@@ -15192,7 +15194,7 @@
     </row>
     <row r="108">
       <c r="A108" t="s" s="2">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="B108" t="s" s="2">
         <v>437</v>
@@ -15310,7 +15312,7 @@
     </row>
     <row r="109">
       <c r="A109" t="s" s="2">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="B109" t="s" s="2">
         <v>438</v>
@@ -15430,7 +15432,7 @@
     </row>
     <row r="110">
       <c r="A110" t="s" s="2">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="B110" t="s" s="2">
         <v>439</v>
@@ -15552,7 +15554,7 @@
     </row>
     <row r="111">
       <c r="A111" t="s" s="2">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B111" t="s" s="2">
         <v>440</v>
@@ -15600,7 +15602,7 @@
         <v>20</v>
       </c>
       <c r="S111" t="s" s="2">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="T111" t="s" s="2">
         <v>20</v>
@@ -15674,7 +15676,7 @@
     </row>
     <row r="112">
       <c r="A112" t="s" s="2">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="B112" t="s" s="2">
         <v>445</v>
@@ -15700,7 +15702,7 @@
         <v>92</v>
       </c>
       <c r="K112" t="s" s="2">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="L112" t="s" s="2">
         <v>446</v>
@@ -15796,7 +15798,7 @@
     </row>
     <row r="113">
       <c r="A113" t="s" s="2">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="B113" t="s" s="2">
         <v>449</v>
@@ -15918,7 +15920,7 @@
     </row>
     <row r="114">
       <c r="A114" t="s" s="2">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="B114" t="s" s="2">
         <v>453</v>
@@ -16040,7 +16042,7 @@
     </row>
     <row r="115">
       <c r="A115" t="s" s="2">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="B115" t="s" s="2">
         <v>454</v>
@@ -16162,13 +16164,13 @@
     </row>
     <row r="116">
       <c r="A116" t="s" s="2">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="B116" t="s" s="2">
         <v>427</v>
       </c>
       <c r="C116" t="s" s="2">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="D116" t="s" s="2">
         <v>20</v>
@@ -16286,7 +16288,7 @@
     </row>
     <row r="117">
       <c r="A117" t="s" s="2">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="B117" t="s" s="2">
         <v>437</v>
@@ -16404,7 +16406,7 @@
     </row>
     <row r="118">
       <c r="A118" t="s" s="2">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="B118" t="s" s="2">
         <v>438</v>
@@ -16524,7 +16526,7 @@
     </row>
     <row r="119">
       <c r="A119" t="s" s="2">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="B119" t="s" s="2">
         <v>439</v>
@@ -16646,7 +16648,7 @@
     </row>
     <row r="120">
       <c r="A120" t="s" s="2">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B120" t="s" s="2">
         <v>440</v>
@@ -16694,7 +16696,7 @@
         <v>20</v>
       </c>
       <c r="S120" t="s" s="2">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="T120" t="s" s="2">
         <v>20</v>
@@ -16768,7 +16770,7 @@
     </row>
     <row r="121">
       <c r="A121" t="s" s="2">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B121" t="s" s="2">
         <v>445</v>
@@ -16794,7 +16796,7 @@
         <v>92</v>
       </c>
       <c r="K121" t="s" s="2">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="L121" t="s" s="2">
         <v>446</v>
@@ -16890,7 +16892,7 @@
     </row>
     <row r="122">
       <c r="A122" t="s" s="2">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="B122" t="s" s="2">
         <v>449</v>
@@ -17012,7 +17014,7 @@
     </row>
     <row r="123">
       <c r="A123" t="s" s="2">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="B123" t="s" s="2">
         <v>453</v>
@@ -17134,7 +17136,7 @@
     </row>
     <row r="124">
       <c r="A124" t="s" s="2">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="B124" t="s" s="2">
         <v>454</v>
@@ -17256,13 +17258,13 @@
     </row>
     <row r="125">
       <c r="A125" t="s" s="2">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B125" t="s" s="2">
         <v>427</v>
       </c>
       <c r="C125" t="s" s="2">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="D125" t="s" s="2">
         <v>20</v>
@@ -17380,7 +17382,7 @@
     </row>
     <row r="126">
       <c r="A126" t="s" s="2">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="B126" t="s" s="2">
         <v>437</v>
@@ -17498,7 +17500,7 @@
     </row>
     <row r="127">
       <c r="A127" t="s" s="2">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="B127" t="s" s="2">
         <v>438</v>
@@ -17618,7 +17620,7 @@
     </row>
     <row r="128">
       <c r="A128" t="s" s="2">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="B128" t="s" s="2">
         <v>439</v>
@@ -17740,7 +17742,7 @@
     </row>
     <row r="129">
       <c r="A129" t="s" s="2">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="B129" t="s" s="2">
         <v>440</v>
@@ -17788,7 +17790,7 @@
         <v>20</v>
       </c>
       <c r="S129" t="s" s="2">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="T129" t="s" s="2">
         <v>20</v>
@@ -17862,7 +17864,7 @@
     </row>
     <row r="130">
       <c r="A130" t="s" s="2">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="B130" t="s" s="2">
         <v>445</v>
@@ -17984,7 +17986,7 @@
     </row>
     <row r="131">
       <c r="A131" t="s" s="2">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="B131" t="s" s="2">
         <v>449</v>
@@ -18106,7 +18108,7 @@
     </row>
     <row r="132">
       <c r="A132" t="s" s="2">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="B132" t="s" s="2">
         <v>453</v>
@@ -18228,7 +18230,7 @@
     </row>
     <row r="133">
       <c r="A133" t="s" s="2">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="B133" t="s" s="2">
         <v>454</v>
@@ -18350,13 +18352,13 @@
     </row>
     <row r="134">
       <c r="A134" t="s" s="2">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="B134" t="s" s="2">
         <v>427</v>
       </c>
       <c r="C134" t="s" s="2">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="D134" t="s" s="2">
         <v>20</v>
@@ -18474,7 +18476,7 @@
     </row>
     <row r="135">
       <c r="A135" t="s" s="2">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="B135" t="s" s="2">
         <v>437</v>
@@ -18592,7 +18594,7 @@
     </row>
     <row r="136">
       <c r="A136" t="s" s="2">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B136" t="s" s="2">
         <v>438</v>
@@ -18712,7 +18714,7 @@
     </row>
     <row r="137">
       <c r="A137" t="s" s="2">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="B137" t="s" s="2">
         <v>439</v>
@@ -18834,7 +18836,7 @@
     </row>
     <row r="138">
       <c r="A138" t="s" s="2">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="B138" t="s" s="2">
         <v>440</v>
@@ -18882,7 +18884,7 @@
         <v>20</v>
       </c>
       <c r="S138" t="s" s="2">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="T138" t="s" s="2">
         <v>20</v>
@@ -18956,7 +18958,7 @@
     </row>
     <row r="139">
       <c r="A139" t="s" s="2">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="B139" t="s" s="2">
         <v>445</v>
@@ -19078,7 +19080,7 @@
     </row>
     <row r="140">
       <c r="A140" t="s" s="2">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="B140" t="s" s="2">
         <v>449</v>
@@ -19200,7 +19202,7 @@
     </row>
     <row r="141">
       <c r="A141" t="s" s="2">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="B141" t="s" s="2">
         <v>453</v>
@@ -19322,7 +19324,7 @@
     </row>
     <row r="142">
       <c r="A142" t="s" s="2">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="B142" t="s" s="2">
         <v>454</v>
@@ -19444,13 +19446,13 @@
     </row>
     <row r="143">
       <c r="A143" t="s" s="2">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="B143" t="s" s="2">
         <v>427</v>
       </c>
       <c r="C143" t="s" s="2">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="D143" t="s" s="2">
         <v>20</v>
@@ -19568,7 +19570,7 @@
     </row>
     <row r="144">
       <c r="A144" t="s" s="2">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="B144" t="s" s="2">
         <v>437</v>
@@ -19686,7 +19688,7 @@
     </row>
     <row r="145">
       <c r="A145" t="s" s="2">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="B145" t="s" s="2">
         <v>438</v>
@@ -19806,7 +19808,7 @@
     </row>
     <row r="146">
       <c r="A146" t="s" s="2">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="B146" t="s" s="2">
         <v>439</v>
@@ -19928,7 +19930,7 @@
     </row>
     <row r="147">
       <c r="A147" t="s" s="2">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="B147" t="s" s="2">
         <v>440</v>
@@ -19976,7 +19978,7 @@
         <v>20</v>
       </c>
       <c r="S147" t="s" s="2">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="T147" t="s" s="2">
         <v>20</v>
@@ -20050,7 +20052,7 @@
     </row>
     <row r="148">
       <c r="A148" t="s" s="2">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="B148" t="s" s="2">
         <v>445</v>
@@ -20172,7 +20174,7 @@
     </row>
     <row r="149">
       <c r="A149" t="s" s="2">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="B149" t="s" s="2">
         <v>449</v>
@@ -20294,7 +20296,7 @@
     </row>
     <row r="150">
       <c r="A150" t="s" s="2">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="B150" t="s" s="2">
         <v>453</v>
@@ -20416,7 +20418,7 @@
     </row>
     <row r="151">
       <c r="A151" t="s" s="2">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="B151" t="s" s="2">
         <v>454</v>

</xml_diff>